<commit_message>
Datasets and code for the flora comparison between 1980 and 2019
</commit_message>
<xml_diff>
--- a/Rabinowitz_Rapp_1980_SR_Data.xlsx
+++ b/Rabinowitz_Rapp_1980_SR_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wynnekat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{888DC22D-B6CE-A646-8541-CFF8F1D197DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEE21D6-CD8D-E443-A223-E3CD2B84F6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17480" yWindow="740" windowWidth="16220" windowHeight="17260" xr2:uid="{CC9EF903-B324-8A42-BE14-AD7AB7BE9681}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>